<commit_message>
feat: implemented transportation impacts
</commit_message>
<xml_diff>
--- a/references/background_data/a4_emissions.xlsx
+++ b/references/background_data/a4_emissions.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mchaf\Documents\GitHub_CLF\pod_lca_data_analysis\references\background_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{39C4C57E-3222-4E8E-95BF-AD6BC85BA9AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{268C8533-479E-4325-B00D-30236A9B2912}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11205"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="a4_emissions" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>Product system name</t>
   </si>
@@ -34,9 +34,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Transport, aircraft, freight</t>
-  </si>
-  <si>
     <t>1 tkm</t>
   </si>
   <si>
@@ -55,59 +52,32 @@
     <t>Transport, ocean freighter, average fuel mix</t>
   </si>
   <si>
-    <t>Transport, light commercial truck, diesel powered</t>
-  </si>
-  <si>
-    <t>More specific truck entries (do not implement these for now)</t>
-  </si>
-  <si>
-    <t>Transport, light commercial truck, gasoline powered</t>
-  </si>
-  <si>
-    <t>Transport, single unit truck, diesel powered</t>
-  </si>
-  <si>
-    <t>Transport, single unit truck, gasoline powered</t>
-  </si>
-  <si>
-    <t>Transport, single unit truck, long-haul, diesel powered</t>
-  </si>
-  <si>
-    <t>Transport, single unit truck, long-haul, gasoline powered</t>
-  </si>
-  <si>
-    <t>Transport, single unit truck, short-haul, diesel powered</t>
-  </si>
-  <si>
-    <t>Transport, single unit truck, short-haul, gasoline powered</t>
-  </si>
-  <si>
-    <t>Acidification Potential</t>
-  </si>
-  <si>
-    <t>Eutrophication Potential</t>
-  </si>
-  <si>
-    <t>Global Warming Potential_fossil</t>
-  </si>
-  <si>
-    <t>Smog Formation Potential</t>
-  </si>
-  <si>
-    <t>Ozone Depletion Potential</t>
-  </si>
-  <si>
-    <t>Global Warming Potential_biogenic</t>
-  </si>
-  <si>
-    <t>Global Warming Potential_luluc</t>
+    <t>acp</t>
+  </si>
+  <si>
+    <t>eup</t>
+  </si>
+  <si>
+    <t>odp</t>
+  </si>
+  <si>
+    <t>smg</t>
+  </si>
+  <si>
+    <t>GWPf</t>
+  </si>
+  <si>
+    <t>GWPb</t>
+  </si>
+  <si>
+    <t>GWP-LULUC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,6 +211,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCCCCCC"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="33">
@@ -584,9 +566,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -941,11 +929,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,25 +946,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="F1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="G1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="H1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="I1" t="s">
         <v>1</v>
@@ -990,28 +978,28 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1">
+        <v>3.5199999999999999E-4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1.73E-5</v>
+      </c>
+      <c r="D2">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>2.0000000000000001E-10</v>
+      </c>
+      <c r="H2" s="1">
+        <v>9.6100000000000005E-3</v>
+      </c>
+      <c r="I2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1">
-        <v>5.0400000000000002E-3</v>
-      </c>
-      <c r="C2" s="1">
-        <v>3.0200000000000002E-4</v>
-      </c>
-      <c r="D2">
-        <v>1.2490000000000001</v>
-      </c>
-      <c r="G2" s="1">
-        <v>8.1799999999999995E-9</v>
-      </c>
-      <c r="H2" s="1">
-        <v>0.16400000000000001</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>5</v>
-      </c>
-      <c r="J2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1019,25 +1007,25 @@
         <v>7</v>
       </c>
       <c r="B3" s="1">
-        <v>3.5199999999999999E-4</v>
+        <v>3.7399999999999998E-4</v>
       </c>
       <c r="C3" s="1">
-        <v>1.73E-5</v>
+        <v>2.3099999999999999E-5</v>
       </c>
       <c r="D3">
-        <v>3.4000000000000002E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="G3" s="1">
-        <v>2.0000000000000001E-10</v>
+        <v>1.35E-10</v>
       </c>
       <c r="H3" s="1">
-        <v>9.6100000000000005E-3</v>
+        <v>1.29E-2</v>
       </c>
       <c r="I3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" t="s">
         <v>5</v>
-      </c>
-      <c r="J3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1045,25 +1033,25 @@
         <v>8</v>
       </c>
       <c r="B4" s="1">
-        <v>3.7399999999999998E-4</v>
+        <v>4.8000000000000001E-4</v>
       </c>
       <c r="C4" s="1">
-        <v>2.3099999999999999E-5</v>
+        <v>2.8E-5</v>
       </c>
       <c r="D4">
-        <v>2.1999999999999999E-2</v>
+        <v>9.4E-2</v>
       </c>
       <c r="G4" s="1">
-        <v>1.35E-10</v>
+        <v>5.68E-10</v>
       </c>
       <c r="H4" s="1">
-        <v>1.29E-2</v>
+        <v>1.54E-2</v>
       </c>
       <c r="I4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" t="s">
         <v>5</v>
-      </c>
-      <c r="J4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1071,286 +1059,50 @@
         <v>9</v>
       </c>
       <c r="B5" s="1">
-        <v>4.8000000000000001E-4</v>
+        <v>3.6499999999999998E-4</v>
       </c>
       <c r="C5" s="1">
-        <v>2.8E-5</v>
+        <v>2.0000000000000002E-5</v>
       </c>
       <c r="D5">
-        <v>9.4E-2</v>
+        <v>1.9E-2</v>
       </c>
       <c r="G5" s="1">
-        <v>5.68E-10</v>
+        <v>1.11E-10</v>
       </c>
       <c r="H5" s="1">
-        <v>1.54E-2</v>
+        <v>1.12E-2</v>
       </c>
       <c r="I5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" t="s">
         <v>5</v>
       </c>
-      <c r="J5" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1">
-        <v>3.6499999999999998E-4</v>
-      </c>
-      <c r="C6" s="1">
-        <v>2.0000000000000002E-5</v>
-      </c>
-      <c r="D6">
-        <v>1.9E-2</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1.11E-10</v>
-      </c>
-      <c r="H6" s="1">
-        <v>1.12E-2</v>
-      </c>
-      <c r="I6" t="s">
-        <v>5</v>
-      </c>
-      <c r="J6" t="s">
-        <v>6</v>
-      </c>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C15" s="2"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="1">
-        <v>7.77E-3</v>
-      </c>
-      <c r="C7" s="1">
-        <v>4.73E-4</v>
-      </c>
-      <c r="D7">
-        <v>0.88900000000000001</v>
-      </c>
-      <c r="G7" s="1">
-        <v>5.9200000000000002E-9</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0.25900000000000001</v>
-      </c>
-      <c r="I7" t="s">
-        <v>5</v>
-      </c>
-      <c r="J7" t="s">
-        <v>6</v>
-      </c>
-      <c r="K7" t="s">
-        <v>12</v>
-      </c>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C16" s="3"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="1">
-        <v>3.5000000000000001E-3</v>
-      </c>
-      <c r="C8" s="1">
-        <v>2.0799999999999999E-4</v>
-      </c>
-      <c r="D8">
-        <v>0.66900000000000004</v>
-      </c>
-      <c r="G8" s="1">
-        <v>4.2400000000000002E-9</v>
-      </c>
-      <c r="H8" s="1">
-        <v>0.115</v>
-      </c>
-      <c r="I8" t="s">
-        <v>5</v>
-      </c>
-      <c r="J8" t="s">
-        <v>6</v>
-      </c>
-      <c r="K8" t="s">
-        <v>12</v>
-      </c>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="3"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="1">
-        <v>1.08E-3</v>
-      </c>
-      <c r="C9" s="1">
-        <v>6.3499999999999999E-5</v>
-      </c>
-      <c r="D9">
-        <v>0.20200000000000001</v>
-      </c>
-      <c r="G9" s="1">
-        <v>1.2199999999999999E-9</v>
-      </c>
-      <c r="H9" s="1">
-        <v>3.5099999999999999E-2</v>
-      </c>
-      <c r="I9" t="s">
-        <v>5</v>
-      </c>
-      <c r="J9" t="s">
-        <v>6</v>
-      </c>
-      <c r="K9" t="s">
-        <v>12</v>
-      </c>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="3"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="1">
-        <v>7.3700000000000002E-4</v>
-      </c>
-      <c r="C10" s="1">
-        <v>4.2500000000000003E-5</v>
-      </c>
-      <c r="D10">
-        <v>0.16</v>
-      </c>
-      <c r="G10" s="1">
-        <v>1.0399999999999999E-9</v>
-      </c>
-      <c r="H10" s="1">
-        <v>2.3900000000000001E-2</v>
-      </c>
-      <c r="I10" t="s">
-        <v>5</v>
-      </c>
-      <c r="J10" t="s">
-        <v>6</v>
-      </c>
-      <c r="K10" t="s">
-        <v>12</v>
-      </c>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="3"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="1">
-        <v>2.8500000000000001E-3</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1.74E-4</v>
-      </c>
-      <c r="D11">
-        <v>0.38900000000000001</v>
-      </c>
-      <c r="G11" s="1">
-        <v>2.6200000000000001E-9</v>
-      </c>
-      <c r="H11" s="1">
-        <v>9.4799999999999995E-2</v>
-      </c>
-      <c r="I11" t="s">
-        <v>5</v>
-      </c>
-      <c r="J11" t="s">
-        <v>6</v>
-      </c>
-      <c r="K11" t="s">
-        <v>12</v>
-      </c>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="3"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="1">
-        <v>2.2399999999999998E-3</v>
-      </c>
-      <c r="C12" s="1">
-        <v>1.34E-4</v>
-      </c>
-      <c r="D12">
-        <v>0.38900000000000001</v>
-      </c>
-      <c r="G12" s="1">
-        <v>2.4899999999999999E-9</v>
-      </c>
-      <c r="H12" s="1">
-        <v>7.3800000000000004E-2</v>
-      </c>
-      <c r="I12" t="s">
-        <v>5</v>
-      </c>
-      <c r="J12" t="s">
-        <v>6</v>
-      </c>
-      <c r="K12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="1">
-        <v>2.48E-3</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1.4999999999999999E-4</v>
-      </c>
-      <c r="D13">
-        <v>0.32200000000000001</v>
-      </c>
-      <c r="G13" s="1">
-        <v>2.1400000000000001E-9</v>
-      </c>
-      <c r="H13" s="1">
-        <v>8.1699999999999995E-2</v>
-      </c>
-      <c r="I13" t="s">
-        <v>5</v>
-      </c>
-      <c r="J13" t="s">
-        <v>6</v>
-      </c>
-      <c r="K13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="1">
-        <v>1.92E-3</v>
-      </c>
-      <c r="C14" s="1">
-        <v>1.15E-4</v>
-      </c>
-      <c r="D14">
-        <v>0.316</v>
-      </c>
-      <c r="G14" s="1">
-        <v>2.0099999999999999E-9</v>
-      </c>
-      <c r="H14" s="1">
-        <v>6.4299999999999996E-2</v>
-      </c>
-      <c r="I14" t="s">
-        <v>5</v>
-      </c>
-      <c r="J14" t="s">
-        <v>6</v>
-      </c>
-      <c r="K14" t="s">
-        <v>12</v>
-      </c>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: transportation impact updates for removing columns
</commit_message>
<xml_diff>
--- a/references/background_data/a4_emissions.xlsx
+++ b/references/background_data/a4_emissions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mchaf\Documents\GitHub_CLF\pod_lca_data_analysis\references\background_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{268C8533-479E-4325-B00D-30236A9B2912}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E317F989-037D-4E7D-9A22-81A0A8630D26}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -933,7 +933,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,6 +989,12 @@
       <c r="D2">
         <v>3.4000000000000002E-2</v>
       </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
       <c r="G2" s="1">
         <v>2.0000000000000001E-10</v>
       </c>
@@ -1015,6 +1021,12 @@
       <c r="D3">
         <v>2.1999999999999999E-2</v>
       </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
       <c r="G3" s="1">
         <v>1.35E-10</v>
       </c>
@@ -1041,6 +1053,12 @@
       <c r="D4">
         <v>9.4E-2</v>
       </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
       <c r="G4" s="1">
         <v>5.68E-10</v>
       </c>
@@ -1066,6 +1084,12 @@
       </c>
       <c r="D5">
         <v>1.9E-2</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
       </c>
       <c r="G5" s="1">
         <v>1.11E-10</v>

</xml_diff>

<commit_message>
feat: add stored carbon to all background data
</commit_message>
<xml_diff>
--- a/references/background_data/a4_emissions.xlsx
+++ b/references/background_data/a4_emissions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mchaf\Documents\GitHub_CLF\pod_lca_data_analysis\references\background_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49FE828-DFAA-437D-A220-851734E023A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A56EBBC-2457-4A9F-BCBF-3F24DE97B0D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>Product system name</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>GWP-LULUC</t>
+  </si>
+  <si>
+    <t>stored_carbon</t>
   </si>
 </sst>
 </file>
@@ -927,10 +930,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G2" sqref="G2:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -938,7 +941,7 @@
     <col min="1" max="1" width="53" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -958,19 +961,22 @@
         <v>15</v>
       </c>
       <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>1</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -989,20 +995,23 @@
       <c r="F2">
         <v>0</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
         <v>2.0000000000000001E-10</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>9.6100000000000005E-3</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>3</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1021,20 +1030,23 @@
       <c r="F3">
         <v>0</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
         <v>1.35E-10</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>1.29E-2</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>3</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1053,20 +1065,23 @@
       <c r="F4">
         <v>0</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
         <v>5.68E-10</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>1.54E-2</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>3</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1085,23 +1100,26 @@
       <c r="F5">
         <v>0</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
         <v>1.11E-10</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>1.12E-2</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>3</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C16" s="3"/>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">

</xml_diff>